<commit_message>
V2 - added statistics and Month/Year map views
</commit_message>
<xml_diff>
--- a/gpstracker_languages.xlsx
+++ b/gpstracker_languages.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="308">
   <si>
     <t>COMMENT</t>
   </si>
@@ -502,19 +502,181 @@
     <t>Поездок пока нет.</t>
   </si>
   <si>
+    <t>map_all_drives</t>
+  </si>
+  <si>
+    <t>All drives</t>
+  </si>
+  <si>
+    <t>Visi braucieni</t>
+  </si>
+  <si>
+    <t>Все поездки</t>
+  </si>
+  <si>
     <t>#STATS</t>
   </si>
   <si>
-    <t>stats_no_data</t>
-  </si>
-  <si>
-    <t>Statistics will appear here..\n\n\nOnce I finish programming this.</t>
-  </si>
-  <si>
-    <t>Šeit parādīsies statistika..\n\n\nKad pabeigšu programmēt šo.</t>
-  </si>
-  <si>
-    <t>Здесь появится статистика..\n\n\nКак только я закончу это программировать.</t>
+    <t>stats_drives_days_in_year</t>
+  </si>
+  <si>
+    <t>xxx days (yyy drives) in a year</t>
+  </si>
+  <si>
+    <t>xxx dienas (yyy braucieni) gadā</t>
+  </si>
+  <si>
+    <t>xxx дней (yyy поездок) в год</t>
+  </si>
+  <si>
+    <t>stats_drives_days_in_week</t>
+  </si>
+  <si>
+    <t>xxx days (yyy drives) ~ in a week</t>
+  </si>
+  <si>
+    <t>xxx dienas (yyy braucieni) ~ nedēļā</t>
+  </si>
+  <si>
+    <t>xxx дней (yyy поездок) ~ в неделю</t>
+  </si>
+  <si>
+    <t>stats_drives_days_in_month</t>
+  </si>
+  <si>
+    <t>xxx days (yyy drives) ~ in a month</t>
+  </si>
+  <si>
+    <t>xxx dienas (yyy braucieni) ~ mēnesī</t>
+  </si>
+  <si>
+    <t>xxx дней (yyy поездок) ~ в месяц</t>
+  </si>
+  <si>
+    <t>stats_avg_month_eur</t>
+  </si>
+  <si>
+    <t>~ xxx Eur per month</t>
+  </si>
+  <si>
+    <t>~ mēnesī xxx Eur</t>
+  </si>
+  <si>
+    <t>~ xxx евро в месяц</t>
+  </si>
+  <si>
+    <t>stats_avg_half_year_eur</t>
+  </si>
+  <si>
+    <t>~ xxx Eur per half year</t>
+  </si>
+  <si>
+    <t>~ pusgadā xxx Eur</t>
+  </si>
+  <si>
+    <t>~ xxx евро за полгода</t>
+  </si>
+  <si>
+    <t>stats_avg_year_eur</t>
+  </si>
+  <si>
+    <t>~ xxx Eur per year</t>
+  </si>
+  <si>
+    <t>~ gadā xxx Eur</t>
+  </si>
+  <si>
+    <t>~ xxx евро в год</t>
+  </si>
+  <si>
+    <t>stats_year_interval</t>
+  </si>
+  <si>
+    <t>Year interval</t>
+  </si>
+  <si>
+    <t>Annual interval</t>
+  </si>
+  <si>
+    <t>Годовой интервал</t>
+  </si>
+  <si>
+    <t>stats_first_year</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Pirmais</t>
+  </si>
+  <si>
+    <t>Первый</t>
+  </si>
+  <si>
+    <t>stats_last_year</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>Pēdējais</t>
+  </si>
+  <si>
+    <t>Прошлой</t>
+  </si>
+  <si>
+    <t>stats_average_year</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Vidēji</t>
+  </si>
+  <si>
+    <t>Средний</t>
+  </si>
+  <si>
+    <t>stats_my_car</t>
+  </si>
+  <si>
+    <t>My car</t>
+  </si>
+  <si>
+    <t>Mans auto</t>
+  </si>
+  <si>
+    <t>Моя машина</t>
+  </si>
+  <si>
+    <t>stats_citybee</t>
+  </si>
+  <si>
+    <t>CityBee</t>
+  </si>
+  <si>
+    <t>stats_bolt_drive</t>
+  </si>
+  <si>
+    <t>Bolt Drive</t>
+  </si>
+  <si>
+    <t>stats_carguru</t>
+  </si>
+  <si>
+    <t>CarGuru</t>
+  </si>
+  <si>
+    <t>stats_mixed</t>
+  </si>
+  <si>
+    <t>Mixed</t>
+  </si>
+  <si>
+    <t>Jauktais</t>
+  </si>
+  <si>
+    <t>Смешанный</t>
   </si>
   <si>
     <t>#DEBUG TEXTS</t>
@@ -2091,7 +2253,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2749,484 +2911,604 @@
       </c>
     </row>
     <row r="45" ht="16.6" customHeight="1">
-      <c r="A45" t="s" s="9">
+      <c r="A45" s="8"/>
+      <c r="B45" t="s" s="7">
         <v>163</v>
       </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="11"/>
+      <c r="C45" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="D45" t="s" s="7">
+        <v>165</v>
+      </c>
+      <c r="E45" t="s" s="7">
+        <v>166</v>
+      </c>
     </row>
     <row r="46" ht="16.6" customHeight="1">
-      <c r="A46" s="8"/>
-      <c r="B46" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="C46" t="s" s="7">
-        <v>165</v>
-      </c>
-      <c r="D46" t="s" s="7">
-        <v>166</v>
-      </c>
-      <c r="E46" t="s" s="7">
+      <c r="A46" t="s" s="9">
         <v>167</v>
       </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="11"/>
     </row>
     <row r="47" ht="16.6" customHeight="1">
-      <c r="A47" t="s" s="9">
+      <c r="A47" s="8"/>
+      <c r="B47" t="s" s="7">
         <v>168</v>
       </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="11"/>
+      <c r="C47" t="s" s="7">
+        <v>169</v>
+      </c>
+      <c r="D47" t="s" s="7">
+        <v>170</v>
+      </c>
+      <c r="E47" t="s" s="7">
+        <v>171</v>
+      </c>
     </row>
     <row r="48" ht="16.6" customHeight="1">
       <c r="A48" s="8"/>
       <c r="B48" t="s" s="7">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C48" t="s" s="7">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D48" t="s" s="7">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E48" t="s" s="7">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" ht="16.6" customHeight="1">
       <c r="A49" s="8"/>
       <c r="B49" t="s" s="7">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C49" t="s" s="7">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D49" t="s" s="7">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E49" t="s" s="7">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" ht="16.6" customHeight="1">
       <c r="A50" s="8"/>
       <c r="B50" t="s" s="7">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C50" t="s" s="7">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D50" t="s" s="7">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E50" t="s" s="7">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="51" ht="16.6" customHeight="1">
       <c r="A51" s="8"/>
       <c r="B51" t="s" s="7">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C51" t="s" s="7">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D51" t="s" s="7">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E51" t="s" s="7">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="52" ht="16.6" customHeight="1">
       <c r="A52" s="8"/>
       <c r="B52" t="s" s="7">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C52" t="s" s="7">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D52" t="s" s="7">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E52" t="s" s="7">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" ht="16.6" customHeight="1">
       <c r="A53" s="8"/>
       <c r="B53" t="s" s="7">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C53" t="s" s="7">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D53" t="s" s="7">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E53" t="s" s="7">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" ht="16.6" customHeight="1">
       <c r="A54" s="8"/>
       <c r="B54" t="s" s="7">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C54" t="s" s="7">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D54" t="s" s="7">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E54" t="s" s="7">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="55" ht="16.6" customHeight="1">
       <c r="A55" s="8"/>
       <c r="B55" t="s" s="7">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C55" t="s" s="7">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D55" t="s" s="7">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E55" t="s" s="7">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="56" ht="16.6" customHeight="1">
       <c r="A56" s="8"/>
       <c r="B56" t="s" s="7">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C56" t="s" s="7">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D56" t="s" s="7">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E56" t="s" s="7">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="57" ht="17" customHeight="1">
-      <c r="A57" t="s" s="9">
-        <v>205</v>
-      </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="11"/>
-    </row>
-    <row r="58" ht="17" customHeight="1">
-      <c r="A58" s="14"/>
-      <c r="B58" t="s" s="15">
-        <v>206</v>
-      </c>
-      <c r="C58" t="s" s="15">
         <v>207</v>
       </c>
-      <c r="D58" t="s" s="15">
+    </row>
+    <row r="57" ht="16.6" customHeight="1">
+      <c r="A57" s="8"/>
+      <c r="B57" t="s" s="7">
         <v>208</v>
       </c>
-      <c r="E58" t="s" s="15">
+      <c r="C57" t="s" s="7">
         <v>209</v>
       </c>
-    </row>
-    <row r="59" ht="17" customHeight="1">
-      <c r="A59" s="14"/>
-      <c r="B59" t="s" s="15">
+      <c r="D57" t="s" s="7">
         <v>210</v>
       </c>
-      <c r="C59" t="s" s="15">
+      <c r="E57" t="s" s="7">
         <v>211</v>
       </c>
-      <c r="D59" t="s" s="15">
+    </row>
+    <row r="58" ht="16.6" customHeight="1">
+      <c r="A58" s="8"/>
+      <c r="B58" t="s" s="7">
         <v>212</v>
       </c>
-      <c r="E59" t="s" s="15">
+      <c r="C58" t="s" s="7">
         <v>213</v>
       </c>
-    </row>
-    <row r="60" ht="17" customHeight="1">
-      <c r="A60" s="14"/>
-      <c r="B60" t="s" s="15">
+      <c r="D58" t="s" s="7">
+        <v>213</v>
+      </c>
+      <c r="E58" t="s" s="7">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="59" ht="16.6" customHeight="1">
+      <c r="A59" s="8"/>
+      <c r="B59" t="s" s="7">
         <v>214</v>
       </c>
-      <c r="C60" t="s" s="15">
+      <c r="C59" t="s" s="7">
         <v>215</v>
       </c>
-      <c r="D60" t="s" s="15">
+      <c r="D59" t="s" s="7">
+        <v>215</v>
+      </c>
+      <c r="E59" t="s" s="7">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="60" ht="16.6" customHeight="1">
+      <c r="A60" s="8"/>
+      <c r="B60" t="s" s="7">
         <v>216</v>
       </c>
-      <c r="E60" t="s" s="15">
+      <c r="C60" t="s" s="7">
         <v>217</v>
       </c>
-    </row>
-    <row r="61" ht="17" customHeight="1">
-      <c r="A61" s="14"/>
-      <c r="B61" t="s" s="15">
+      <c r="D60" t="s" s="7">
+        <v>217</v>
+      </c>
+      <c r="E60" t="s" s="7">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="61" ht="16.6" customHeight="1">
+      <c r="A61" s="8"/>
+      <c r="B61" t="s" s="7">
         <v>218</v>
       </c>
-      <c r="C61" t="s" s="15">
+      <c r="C61" t="s" s="7">
         <v>219</v>
       </c>
-      <c r="D61" t="s" s="15">
+      <c r="D61" t="s" s="7">
         <v>220</v>
       </c>
-      <c r="E61" t="s" s="15">
+      <c r="E61" t="s" s="7">
         <v>221</v>
       </c>
     </row>
-    <row r="62" ht="17" customHeight="1">
-      <c r="A62" s="14"/>
-      <c r="B62" t="s" s="15">
+    <row r="62" ht="16.6" customHeight="1">
+      <c r="A62" t="s" s="9">
         <v>222</v>
       </c>
-      <c r="C62" t="s" s="15">
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="11"/>
+    </row>
+    <row r="63" ht="16.6" customHeight="1">
+      <c r="A63" s="8"/>
+      <c r="B63" t="s" s="7">
         <v>223</v>
       </c>
-      <c r="D62" t="s" s="15">
+      <c r="C63" t="s" s="7">
         <v>224</v>
       </c>
-      <c r="E62" t="s" s="15">
+      <c r="D63" t="s" s="7">
         <v>225</v>
       </c>
-    </row>
-    <row r="63" ht="17" customHeight="1">
-      <c r="A63" s="14"/>
-      <c r="B63" t="s" s="15">
+      <c r="E63" t="s" s="7">
         <v>226</v>
       </c>
-      <c r="C63" t="s" s="15">
+    </row>
+    <row r="64" ht="16.6" customHeight="1">
+      <c r="A64" s="8"/>
+      <c r="B64" t="s" s="7">
         <v>227</v>
       </c>
-      <c r="D63" t="s" s="15">
+      <c r="C64" t="s" s="7">
         <v>228</v>
       </c>
-      <c r="E63" t="s" s="15">
+      <c r="D64" t="s" s="7">
         <v>229</v>
       </c>
-    </row>
-    <row r="64" ht="17" customHeight="1">
-      <c r="A64" s="14"/>
-      <c r="B64" t="s" s="15">
+      <c r="E64" t="s" s="7">
         <v>230</v>
       </c>
-      <c r="C64" t="s" s="15">
+    </row>
+    <row r="65" ht="16.6" customHeight="1">
+      <c r="A65" s="8"/>
+      <c r="B65" t="s" s="7">
         <v>231</v>
       </c>
-      <c r="D64" t="s" s="15">
+      <c r="C65" t="s" s="7">
         <v>232</v>
       </c>
-      <c r="E64" t="s" s="15">
+      <c r="D65" t="s" s="7">
         <v>233</v>
       </c>
-    </row>
-    <row r="65" ht="17" customHeight="1">
-      <c r="A65" s="14"/>
-      <c r="B65" t="s" s="15">
+      <c r="E65" t="s" s="7">
         <v>234</v>
       </c>
-      <c r="C65" t="s" s="15">
+    </row>
+    <row r="66" ht="16.6" customHeight="1">
+      <c r="A66" s="8"/>
+      <c r="B66" t="s" s="7">
         <v>235</v>
       </c>
-      <c r="D65" t="s" s="15">
+      <c r="C66" t="s" s="7">
         <v>236</v>
       </c>
-      <c r="E65" t="s" s="15">
+      <c r="D66" t="s" s="7">
         <v>237</v>
       </c>
-    </row>
-    <row r="66" ht="17" customHeight="1">
-      <c r="A66" s="14"/>
-      <c r="B66" t="s" s="15">
+      <c r="E66" t="s" s="7">
         <v>238</v>
       </c>
-      <c r="C66" t="s" s="15">
+    </row>
+    <row r="67" ht="16.6" customHeight="1">
+      <c r="A67" s="8"/>
+      <c r="B67" t="s" s="7">
         <v>239</v>
       </c>
-      <c r="D66" t="s" s="15">
+      <c r="C67" t="s" s="7">
         <v>240</v>
       </c>
-      <c r="E66" t="s" s="15">
+      <c r="D67" t="s" s="7">
         <v>241</v>
       </c>
-    </row>
-    <row r="67" ht="17" customHeight="1">
-      <c r="A67" s="14"/>
-      <c r="B67" t="s" s="15">
+      <c r="E67" t="s" s="7">
         <v>242</v>
       </c>
-      <c r="C67" t="s" s="15">
+    </row>
+    <row r="68" ht="16.6" customHeight="1">
+      <c r="A68" s="8"/>
+      <c r="B68" t="s" s="7">
         <v>243</v>
       </c>
-      <c r="D67" t="s" s="15">
+      <c r="C68" t="s" s="7">
         <v>244</v>
       </c>
-      <c r="E67" t="s" s="15">
+      <c r="D68" t="s" s="7">
         <v>245</v>
       </c>
-    </row>
-    <row r="68" ht="17" customHeight="1">
-      <c r="A68" s="14"/>
-      <c r="B68" t="s" s="15">
+      <c r="E68" t="s" s="7">
         <v>246</v>
       </c>
-      <c r="C68" t="s" s="15">
+    </row>
+    <row r="69" ht="16.6" customHeight="1">
+      <c r="A69" s="8"/>
+      <c r="B69" t="s" s="7">
         <v>247</v>
       </c>
-      <c r="D68" t="s" s="15">
+      <c r="C69" t="s" s="7">
         <v>248</v>
       </c>
-      <c r="E68" t="s" s="15">
+      <c r="D69" t="s" s="7">
         <v>249</v>
       </c>
-    </row>
-    <row r="69" ht="17" customHeight="1">
-      <c r="A69" s="14"/>
-      <c r="B69" t="s" s="15">
+      <c r="E69" t="s" s="7">
         <v>250</v>
       </c>
-      <c r="C69" t="s" s="15">
+    </row>
+    <row r="70" ht="16.6" customHeight="1">
+      <c r="A70" s="8"/>
+      <c r="B70" t="s" s="7">
         <v>251</v>
       </c>
-      <c r="D69" t="s" s="15">
+      <c r="C70" t="s" s="7">
         <v>252</v>
       </c>
-      <c r="E69" t="s" s="15">
+      <c r="D70" t="s" s="7">
         <v>253</v>
       </c>
-    </row>
-    <row r="70" ht="17" customHeight="1">
-      <c r="A70" s="14"/>
-      <c r="B70" s="15"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
-    </row>
-    <row r="71" ht="17" customHeight="1">
-      <c r="A71" s="14"/>
-      <c r="B71" s="15"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
+      <c r="E70" t="s" s="7">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="71" ht="16.6" customHeight="1">
+      <c r="A71" s="8"/>
+      <c r="B71" t="s" s="7">
+        <v>255</v>
+      </c>
+      <c r="C71" t="s" s="7">
+        <v>256</v>
+      </c>
+      <c r="D71" t="s" s="7">
+        <v>257</v>
+      </c>
+      <c r="E71" t="s" s="7">
+        <v>258</v>
+      </c>
     </row>
     <row r="72" ht="17" customHeight="1">
-      <c r="A72" s="14"/>
-      <c r="B72" s="16"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
+      <c r="A72" t="s" s="9">
+        <v>259</v>
+      </c>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="11"/>
     </row>
     <row r="73" ht="17" customHeight="1">
       <c r="A73" s="14"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
+      <c r="B73" t="s" s="15">
+        <v>260</v>
+      </c>
+      <c r="C73" t="s" s="15">
+        <v>261</v>
+      </c>
+      <c r="D73" t="s" s="15">
+        <v>262</v>
+      </c>
+      <c r="E73" t="s" s="15">
+        <v>263</v>
+      </c>
     </row>
     <row r="74" ht="17" customHeight="1">
       <c r="A74" s="14"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
+      <c r="B74" t="s" s="15">
+        <v>264</v>
+      </c>
+      <c r="C74" t="s" s="15">
+        <v>265</v>
+      </c>
+      <c r="D74" t="s" s="15">
+        <v>266</v>
+      </c>
+      <c r="E74" t="s" s="15">
+        <v>267</v>
+      </c>
     </row>
     <row r="75" ht="17" customHeight="1">
       <c r="A75" s="14"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
+      <c r="B75" t="s" s="15">
+        <v>268</v>
+      </c>
+      <c r="C75" t="s" s="15">
+        <v>269</v>
+      </c>
+      <c r="D75" t="s" s="15">
+        <v>270</v>
+      </c>
+      <c r="E75" t="s" s="15">
+        <v>271</v>
+      </c>
     </row>
     <row r="76" ht="17" customHeight="1">
       <c r="A76" s="14"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
+      <c r="B76" t="s" s="15">
+        <v>272</v>
+      </c>
+      <c r="C76" t="s" s="15">
+        <v>273</v>
+      </c>
+      <c r="D76" t="s" s="15">
+        <v>274</v>
+      </c>
+      <c r="E76" t="s" s="15">
+        <v>275</v>
+      </c>
     </row>
     <row r="77" ht="17" customHeight="1">
       <c r="A77" s="14"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
+      <c r="B77" t="s" s="15">
+        <v>276</v>
+      </c>
+      <c r="C77" t="s" s="15">
+        <v>277</v>
+      </c>
+      <c r="D77" t="s" s="15">
+        <v>278</v>
+      </c>
+      <c r="E77" t="s" s="15">
+        <v>279</v>
+      </c>
     </row>
     <row r="78" ht="17" customHeight="1">
       <c r="A78" s="14"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="14"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
+      <c r="B78" t="s" s="15">
+        <v>280</v>
+      </c>
+      <c r="C78" t="s" s="15">
+        <v>281</v>
+      </c>
+      <c r="D78" t="s" s="15">
+        <v>282</v>
+      </c>
+      <c r="E78" t="s" s="15">
+        <v>283</v>
+      </c>
     </row>
     <row r="79" ht="17" customHeight="1">
       <c r="A79" s="14"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="14"/>
-      <c r="E79" s="14"/>
+      <c r="B79" t="s" s="15">
+        <v>284</v>
+      </c>
+      <c r="C79" t="s" s="15">
+        <v>285</v>
+      </c>
+      <c r="D79" t="s" s="15">
+        <v>286</v>
+      </c>
+      <c r="E79" t="s" s="15">
+        <v>287</v>
+      </c>
     </row>
     <row r="80" ht="17" customHeight="1">
       <c r="A80" s="14"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
+      <c r="B80" t="s" s="15">
+        <v>288</v>
+      </c>
+      <c r="C80" t="s" s="15">
+        <v>289</v>
+      </c>
+      <c r="D80" t="s" s="15">
+        <v>290</v>
+      </c>
+      <c r="E80" t="s" s="15">
+        <v>291</v>
+      </c>
     </row>
     <row r="81" ht="17" customHeight="1">
       <c r="A81" s="14"/>
-      <c r="B81" s="17"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="14"/>
+      <c r="B81" t="s" s="15">
+        <v>292</v>
+      </c>
+      <c r="C81" t="s" s="15">
+        <v>293</v>
+      </c>
+      <c r="D81" t="s" s="15">
+        <v>294</v>
+      </c>
+      <c r="E81" t="s" s="15">
+        <v>295</v>
+      </c>
     </row>
     <row r="82" ht="17" customHeight="1">
       <c r="A82" s="14"/>
-      <c r="B82" s="17"/>
-      <c r="C82" s="14"/>
-      <c r="D82" s="14"/>
-      <c r="E82" s="14"/>
+      <c r="B82" t="s" s="15">
+        <v>296</v>
+      </c>
+      <c r="C82" t="s" s="15">
+        <v>297</v>
+      </c>
+      <c r="D82" t="s" s="15">
+        <v>298</v>
+      </c>
+      <c r="E82" t="s" s="15">
+        <v>299</v>
+      </c>
     </row>
     <row r="83" ht="17" customHeight="1">
       <c r="A83" s="14"/>
-      <c r="B83" s="17"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14"/>
-      <c r="E83" s="14"/>
+      <c r="B83" t="s" s="15">
+        <v>300</v>
+      </c>
+      <c r="C83" t="s" s="15">
+        <v>301</v>
+      </c>
+      <c r="D83" t="s" s="15">
+        <v>302</v>
+      </c>
+      <c r="E83" t="s" s="15">
+        <v>303</v>
+      </c>
     </row>
     <row r="84" ht="17" customHeight="1">
       <c r="A84" s="14"/>
-      <c r="B84" s="17"/>
-      <c r="C84" s="14"/>
-      <c r="D84" s="14"/>
-      <c r="E84" s="14"/>
+      <c r="B84" t="s" s="15">
+        <v>304</v>
+      </c>
+      <c r="C84" t="s" s="15">
+        <v>305</v>
+      </c>
+      <c r="D84" t="s" s="15">
+        <v>306</v>
+      </c>
+      <c r="E84" t="s" s="15">
+        <v>307</v>
+      </c>
     </row>
     <row r="85" ht="17" customHeight="1">
       <c r="A85" s="14"/>
-      <c r="B85" s="17"/>
+      <c r="B85" s="15"/>
       <c r="C85" s="14"/>
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
     </row>
     <row r="86" ht="17" customHeight="1">
       <c r="A86" s="14"/>
-      <c r="B86" s="17"/>
+      <c r="B86" s="15"/>
       <c r="C86" s="14"/>
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
     </row>
     <row r="87" ht="17" customHeight="1">
       <c r="A87" s="14"/>
-      <c r="B87" s="17"/>
+      <c r="B87" s="16"/>
       <c r="C87" s="14"/>
       <c r="D87" s="14"/>
       <c r="E87" s="14"/>
@@ -3643,6 +3925,111 @@
       <c r="C146" s="14"/>
       <c r="D146" s="14"/>
       <c r="E146" s="14"/>
+    </row>
+    <row r="147" ht="17" customHeight="1">
+      <c r="A147" s="14"/>
+      <c r="B147" s="17"/>
+      <c r="C147" s="14"/>
+      <c r="D147" s="14"/>
+      <c r="E147" s="14"/>
+    </row>
+    <row r="148" ht="17" customHeight="1">
+      <c r="A148" s="14"/>
+      <c r="B148" s="17"/>
+      <c r="C148" s="14"/>
+      <c r="D148" s="14"/>
+      <c r="E148" s="14"/>
+    </row>
+    <row r="149" ht="17" customHeight="1">
+      <c r="A149" s="14"/>
+      <c r="B149" s="17"/>
+      <c r="C149" s="14"/>
+      <c r="D149" s="14"/>
+      <c r="E149" s="14"/>
+    </row>
+    <row r="150" ht="17" customHeight="1">
+      <c r="A150" s="14"/>
+      <c r="B150" s="17"/>
+      <c r="C150" s="14"/>
+      <c r="D150" s="14"/>
+      <c r="E150" s="14"/>
+    </row>
+    <row r="151" ht="17" customHeight="1">
+      <c r="A151" s="14"/>
+      <c r="B151" s="17"/>
+      <c r="C151" s="14"/>
+      <c r="D151" s="14"/>
+      <c r="E151" s="14"/>
+    </row>
+    <row r="152" ht="17" customHeight="1">
+      <c r="A152" s="14"/>
+      <c r="B152" s="17"/>
+      <c r="C152" s="14"/>
+      <c r="D152" s="14"/>
+      <c r="E152" s="14"/>
+    </row>
+    <row r="153" ht="17" customHeight="1">
+      <c r="A153" s="14"/>
+      <c r="B153" s="17"/>
+      <c r="C153" s="14"/>
+      <c r="D153" s="14"/>
+      <c r="E153" s="14"/>
+    </row>
+    <row r="154" ht="17" customHeight="1">
+      <c r="A154" s="14"/>
+      <c r="B154" s="17"/>
+      <c r="C154" s="14"/>
+      <c r="D154" s="14"/>
+      <c r="E154" s="14"/>
+    </row>
+    <row r="155" ht="17" customHeight="1">
+      <c r="A155" s="14"/>
+      <c r="B155" s="17"/>
+      <c r="C155" s="14"/>
+      <c r="D155" s="14"/>
+      <c r="E155" s="14"/>
+    </row>
+    <row r="156" ht="17" customHeight="1">
+      <c r="A156" s="14"/>
+      <c r="B156" s="17"/>
+      <c r="C156" s="14"/>
+      <c r="D156" s="14"/>
+      <c r="E156" s="14"/>
+    </row>
+    <row r="157" ht="17" customHeight="1">
+      <c r="A157" s="14"/>
+      <c r="B157" s="17"/>
+      <c r="C157" s="14"/>
+      <c r="D157" s="14"/>
+      <c r="E157" s="14"/>
+    </row>
+    <row r="158" ht="17" customHeight="1">
+      <c r="A158" s="14"/>
+      <c r="B158" s="17"/>
+      <c r="C158" s="14"/>
+      <c r="D158" s="14"/>
+      <c r="E158" s="14"/>
+    </row>
+    <row r="159" ht="17" customHeight="1">
+      <c r="A159" s="14"/>
+      <c r="B159" s="17"/>
+      <c r="C159" s="14"/>
+      <c r="D159" s="14"/>
+      <c r="E159" s="14"/>
+    </row>
+    <row r="160" ht="17" customHeight="1">
+      <c r="A160" s="14"/>
+      <c r="B160" s="17"/>
+      <c r="C160" s="14"/>
+      <c r="D160" s="14"/>
+      <c r="E160" s="14"/>
+    </row>
+    <row r="161" ht="17" customHeight="1">
+      <c r="A161" s="14"/>
+      <c r="B161" s="17"/>
+      <c r="C161" s="14"/>
+      <c r="D161" s="14"/>
+      <c r="E161" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
Added a way to move a point in map edit mode
</commit_message>
<xml_diff>
--- a/gpstracker_languages.xlsx
+++ b/gpstracker_languages.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gt/Documents/MainProjects/DrivesApp/SWIFT/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C80DBC-4DF4-9A46-BF8F-318C9E3A5F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="1400" yWindow="500" windowWidth="24720" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lapa1" sheetId="1" r:id="rId4"/>
+    <sheet name="Lapa1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="321">
   <si>
     <t>COMMENT</t>
   </si>
@@ -935,46 +944,75 @@
   </si>
   <si>
     <t>Декабрь</t>
+  </si>
+  <si>
+    <t>done_button_title</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Pabeigt</t>
+  </si>
+  <si>
+    <t>move_button_title</t>
+  </si>
+  <si>
+    <t>Move</t>
+  </si>
+  <si>
+    <t>Pārvietot</t>
+  </si>
+  <si>
+    <t>edit_button_title</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>Labot</t>
+  </si>
+  <si>
+    <t>Сделанный</t>
+  </si>
+  <si>
+    <t>Переместить точку</t>
+  </si>
+  <si>
+    <t>Редактировать</t>
+  </si>
+  <si>
+    <t>Внимание</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1110,64 +1148,30 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1177,25 +1181,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffdaeef3"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFDAEEF3"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1397,7 +1461,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1416,7 +1480,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1446,7 +1510,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1472,7 +1536,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1498,7 +1562,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1524,7 +1588,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1550,7 +1614,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1576,7 +1640,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1602,7 +1666,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1628,7 +1692,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1654,7 +1718,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1667,9 +1731,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1686,7 +1756,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1705,7 +1775,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1731,7 +1801,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1757,7 +1827,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1783,7 +1853,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1809,7 +1879,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1835,7 +1905,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1861,7 +1931,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1887,7 +1957,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1913,7 +1983,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1939,7 +2009,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1952,9 +2022,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1968,7 +2044,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1987,7 +2063,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2017,7 +2093,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2043,7 +2119,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2069,7 +2145,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2095,7 +2171,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2121,7 +2197,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2147,7 +2223,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2173,7 +2249,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2199,7 +2275,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2225,7 +2301,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2238,51 +2314,61 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
-    <col min="2" max="5" width="40.3516" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="2" max="5" width="40.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.6" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="16.6" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4"/>
@@ -2290,1750 +2376,1795 @@
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" ht="16.6" customHeight="1">
-      <c r="A3" t="s" s="6">
+    <row r="3" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s" s="6">
+      <c r="E3" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="16.6" customHeight="1">
-      <c r="A4" t="s" s="7">
+    <row r="4" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s" s="7">
+      <c r="C4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s" s="7">
+      <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s" s="7">
+      <c r="E4" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" ht="16.6" customHeight="1">
-      <c r="A5" t="s" s="7">
+    <row r="5" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s" s="7">
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s" s="7">
+      <c r="C5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s" s="7">
+      <c r="D5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s" s="7">
+      <c r="E5" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" ht="16.6" customHeight="1">
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
-      <c r="B6" t="s" s="7">
+      <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s" s="7">
+      <c r="C6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s" s="7">
+      <c r="D6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s" s="7">
+      <c r="E6" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" ht="16.6" customHeight="1">
+    <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
-      <c r="B7" t="s" s="7">
+      <c r="B7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s" s="7">
+      <c r="C7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s" s="7">
+      <c r="D7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s" s="7">
+      <c r="E7" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" ht="16.6" customHeight="1">
+    <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
-      <c r="B8" t="s" s="7">
+      <c r="B8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s" s="7">
+      <c r="C8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s" s="7">
+      <c r="D8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E8" t="s" s="7">
+      <c r="E8" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" ht="16.6" customHeight="1">
+    <row r="9" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
-      <c r="B9" t="s" s="7">
+      <c r="B9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s" s="7">
+      <c r="C9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D9" t="s" s="7">
+      <c r="D9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E9" t="s" s="7">
+      <c r="E9" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" ht="16.6" customHeight="1">
+    <row r="10" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
-      <c r="B10" t="s" s="7">
+      <c r="B10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s" s="7">
+      <c r="C10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s" s="7">
+      <c r="D10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E10" t="s" s="7">
+      <c r="E10" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" ht="16.6" customHeight="1">
+    <row r="11" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
-      <c r="B11" t="s" s="7">
+      <c r="B11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s" s="7">
+      <c r="C11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D11" t="s" s="7">
+      <c r="D11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E11" t="s" s="7">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" ht="16.6" customHeight="1">
+      <c r="E11" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
-      <c r="B12" t="s" s="7">
+      <c r="B12" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C12" t="s" s="7">
+      <c r="C15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D12" t="s" s="7">
+      <c r="D15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E12" t="s" s="7">
+      <c r="E15" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" ht="16.6" customHeight="1">
-      <c r="A13" t="s" s="9">
+    <row r="16" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" ht="16.6" customHeight="1">
-      <c r="A14" s="8"/>
-      <c r="B14" t="s" s="7">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C14" t="s" s="7">
+      <c r="C17" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D14" t="s" s="7">
+      <c r="D17" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E14" t="s" s="7">
+      <c r="E17" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" ht="16.6" customHeight="1">
-      <c r="A15" s="8"/>
-      <c r="B15" t="s" s="7">
+    <row r="18" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C15" t="s" s="7">
+      <c r="C18" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D15" t="s" s="7">
+      <c r="D18" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E15" t="s" s="7">
+      <c r="E18" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" ht="16.6" customHeight="1">
-      <c r="A16" s="8"/>
-      <c r="B16" t="s" s="7">
+    <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C16" t="s" s="7">
+      <c r="C19" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D16" t="s" s="7">
+      <c r="D19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E16" t="s" s="7">
+      <c r="E19" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" ht="16.6" customHeight="1">
-      <c r="A17" s="12"/>
-      <c r="B17" t="s" s="13">
+    <row r="20" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C17" t="s" s="13">
+      <c r="C20" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D17" t="s" s="13">
+      <c r="D20" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E17" t="s" s="13">
+      <c r="E20" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" ht="16.6" customHeight="1">
-      <c r="A18" t="s" s="3">
+    <row r="21" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" ht="16.6" customHeight="1">
-      <c r="A19" t="s" s="6">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B19" t="s" s="6">
+      <c r="B22" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C19" t="s" s="6">
+      <c r="C22" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D19" t="s" s="6">
+      <c r="D22" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E19" t="s" s="6">
+      <c r="E22" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" ht="16.6" customHeight="1">
-      <c r="A20" s="8"/>
-      <c r="B20" t="s" s="7">
+    <row r="23" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C20" t="s" s="7">
+      <c r="C23" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D20" t="s" s="7">
+      <c r="D23" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E20" t="s" s="7">
+      <c r="E23" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="21" ht="16.6" customHeight="1">
-      <c r="A21" s="8"/>
-      <c r="B21" t="s" s="7">
+    <row r="24" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C21" t="s" s="7">
+      <c r="C24" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D21" t="s" s="7">
+      <c r="D24" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E21" t="s" s="7">
+      <c r="E24" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" ht="16.6" customHeight="1">
-      <c r="A22" s="8"/>
-      <c r="B22" t="s" s="7">
+    <row r="25" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C22" t="s" s="7">
+      <c r="C25" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D22" t="s" s="7">
+      <c r="D25" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E22" t="s" s="7">
+      <c r="E25" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" ht="16.6" customHeight="1">
-      <c r="A23" s="8"/>
-      <c r="B23" t="s" s="7">
+    <row r="26" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C23" t="s" s="7">
+      <c r="C26" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D23" t="s" s="7">
+      <c r="D26" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E23" t="s" s="7">
+      <c r="E26" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="24" ht="16.6" customHeight="1">
-      <c r="A24" s="8"/>
-      <c r="B24" t="s" s="7">
+    <row r="27" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+      <c r="B27" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C24" t="s" s="7">
+      <c r="C27" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D24" t="s" s="7">
+      <c r="D27" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E24" t="s" s="7">
+      <c r="E27" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" ht="16.6" customHeight="1">
-      <c r="A25" s="8"/>
-      <c r="B25" t="s" s="7">
+    <row r="28" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C25" t="s" s="7">
+      <c r="C28" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D25" t="s" s="7">
+      <c r="D28" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E25" t="s" s="7">
+      <c r="E28" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" ht="16.6" customHeight="1">
-      <c r="A26" s="8"/>
-      <c r="B26" t="s" s="7">
+    <row r="29" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+      <c r="B29" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C26" t="s" s="7">
+      <c r="C29" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D26" t="s" s="7">
+      <c r="D29" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E26" t="s" s="7">
+      <c r="E29" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="27" ht="16.6" customHeight="1">
-      <c r="A27" s="8"/>
-      <c r="B27" t="s" s="7">
+    <row r="30" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+      <c r="B30" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C27" t="s" s="7">
+      <c r="C30" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D27" t="s" s="7">
+      <c r="D30" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E27" t="s" s="7">
+      <c r="E30" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" ht="16.6" customHeight="1">
-      <c r="A28" s="8"/>
-      <c r="B28" t="s" s="7">
+    <row r="31" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+      <c r="B31" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C28" t="s" s="7">
+      <c r="C31" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D28" t="s" s="7">
+      <c r="D31" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E28" t="s" s="7">
+      <c r="E31" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="29" ht="16.6" customHeight="1">
-      <c r="A29" s="8"/>
-      <c r="B29" t="s" s="7">
+    <row r="32" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C29" t="s" s="7">
+      <c r="C32" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D29" t="s" s="7">
+      <c r="D32" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E29" t="s" s="7">
+      <c r="E32" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="30" ht="16.6" customHeight="1">
-      <c r="A30" s="8"/>
-      <c r="B30" t="s" s="7">
+    <row r="33" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+      <c r="B33" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C30" t="s" s="7">
+      <c r="C33" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D30" t="s" s="7">
+      <c r="D33" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E30" t="s" s="7">
+      <c r="E33" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="31" ht="16.6" customHeight="1">
-      <c r="A31" s="8"/>
-      <c r="B31" t="s" s="7">
+    <row r="34" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C31" t="s" s="7">
+      <c r="C34" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D31" t="s" s="7">
+      <c r="D34" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E31" t="s" s="7">
+      <c r="E34" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="32" ht="16.6" customHeight="1">
-      <c r="A32" s="8"/>
-      <c r="B32" t="s" s="7">
+    <row r="35" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
+      <c r="B35" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C32" t="s" s="7">
+      <c r="C35" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D32" t="s" s="7">
+      <c r="D35" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E32" t="s" s="7">
+      <c r="E35" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="33" ht="16.6" customHeight="1">
-      <c r="A33" s="8"/>
-      <c r="B33" t="s" s="7">
+    <row r="36" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C33" t="s" s="7">
+      <c r="C36" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D33" t="s" s="7">
+      <c r="D36" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E33" t="s" s="7">
+      <c r="E36" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="34" ht="16.6" customHeight="1">
-      <c r="A34" s="8"/>
-      <c r="B34" t="s" s="7">
+    <row r="37" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="8"/>
+      <c r="B37" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C34" t="s" s="7">
+      <c r="C37" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D34" t="s" s="7">
+      <c r="D37" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E34" t="s" s="7">
+      <c r="E37" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="35" ht="16.6" customHeight="1">
-      <c r="A35" s="8"/>
-      <c r="B35" t="s" s="7">
+    <row r="38" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C35" t="s" s="7">
+      <c r="C38" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D35" t="s" s="7">
+      <c r="D38" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E35" t="s" s="7">
+      <c r="E38" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="36" ht="16.6" customHeight="1">
-      <c r="A36" s="8"/>
-      <c r="B36" t="s" s="7">
+    <row r="39" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="8"/>
+      <c r="B39" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C36" t="s" s="7">
+      <c r="C39" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D36" t="s" s="7">
+      <c r="D39" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E36" t="s" s="7">
+      <c r="E39" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="37" ht="16.6" customHeight="1">
-      <c r="A37" s="8"/>
-      <c r="B37" t="s" s="7">
+    <row r="40" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C37" t="s" s="7">
+      <c r="C40" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D37" t="s" s="7">
+      <c r="D40" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E37" t="s" s="7">
+      <c r="E40" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="38" ht="16.6" customHeight="1">
-      <c r="A38" t="s" s="9">
+    <row r="41" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
-    </row>
-    <row r="39" ht="16.6" customHeight="1">
-      <c r="A39" s="8"/>
-      <c r="B39" t="s" s="7">
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="11"/>
+    </row>
+    <row r="42" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="8"/>
+      <c r="B42" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C39" t="s" s="7">
+      <c r="C42" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D39" t="s" s="7">
+      <c r="D42" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E39" t="s" s="7">
+      <c r="E42" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="40" ht="16.6" customHeight="1">
-      <c r="A40" s="8"/>
-      <c r="B40" t="s" s="7">
+    <row r="43" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="8"/>
+      <c r="B43" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C40" t="s" s="7">
+      <c r="C43" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D40" t="s" s="7">
+      <c r="D43" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E40" t="s" s="7">
+      <c r="E43" s="7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="41" ht="16.6" customHeight="1">
-      <c r="A41" s="8"/>
-      <c r="B41" t="s" s="7">
+    <row r="44" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="8"/>
+      <c r="B44" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C41" t="s" s="7">
+      <c r="C44" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D41" t="s" s="7">
+      <c r="D44" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E41" t="s" s="7">
+      <c r="E44" s="7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="42" ht="16.6" customHeight="1">
-      <c r="A42" s="8"/>
-      <c r="B42" t="s" s="7">
+    <row r="45" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="8"/>
+      <c r="B45" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C42" t="s" s="7">
+      <c r="C45" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D42" t="s" s="7">
+      <c r="D45" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="E42" t="s" s="7">
+      <c r="E45" s="7" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="43" ht="16.6" customHeight="1">
-      <c r="A43" s="8"/>
-      <c r="B43" t="s" s="7">
+    <row r="46" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="8"/>
+      <c r="B46" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C43" t="s" s="7">
+      <c r="C46" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D43" t="s" s="7">
+      <c r="D46" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="E43" t="s" s="7">
+      <c r="E46" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="44" ht="16.6" customHeight="1">
-      <c r="A44" s="8"/>
-      <c r="B44" t="s" s="7">
+    <row r="47" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="8"/>
+      <c r="B47" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C44" t="s" s="7">
+      <c r="C47" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="D44" t="s" s="7">
+      <c r="D47" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="E44" t="s" s="7">
+      <c r="E47" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="45" ht="16.6" customHeight="1">
-      <c r="A45" s="8"/>
-      <c r="B45" t="s" s="7">
+    <row r="48" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="8"/>
+      <c r="B48" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="C45" t="s" s="7">
+      <c r="C48" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="D45" t="s" s="7">
+      <c r="D48" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="E45" t="s" s="7">
+      <c r="E48" s="7" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="46" ht="16.6" customHeight="1">
-      <c r="A46" t="s" s="9">
+    <row r="49" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="11"/>
-    </row>
-    <row r="47" ht="16.6" customHeight="1">
-      <c r="A47" s="8"/>
-      <c r="B47" t="s" s="7">
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="11"/>
+    </row>
+    <row r="50" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8"/>
+      <c r="B50" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="C47" t="s" s="7">
+      <c r="C50" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D47" t="s" s="7">
+      <c r="D50" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="E47" t="s" s="7">
+      <c r="E50" s="7" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="48" ht="16.6" customHeight="1">
-      <c r="A48" s="8"/>
-      <c r="B48" t="s" s="7">
+    <row r="51" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="8"/>
+      <c r="B51" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="C48" t="s" s="7">
+      <c r="C51" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D48" t="s" s="7">
+      <c r="D51" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="E48" t="s" s="7">
+      <c r="E51" s="7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="49" ht="16.6" customHeight="1">
-      <c r="A49" s="8"/>
-      <c r="B49" t="s" s="7">
+    <row r="52" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="8"/>
+      <c r="B52" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="C49" t="s" s="7">
+      <c r="C52" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D49" t="s" s="7">
+      <c r="D52" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E49" t="s" s="7">
+      <c r="E52" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="50" ht="16.6" customHeight="1">
-      <c r="A50" s="8"/>
-      <c r="B50" t="s" s="7">
+    <row r="53" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="8"/>
+      <c r="B53" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="C50" t="s" s="7">
+      <c r="C53" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D50" t="s" s="7">
+      <c r="D53" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="E50" t="s" s="7">
+      <c r="E53" s="7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="51" ht="16.6" customHeight="1">
-      <c r="A51" s="8"/>
-      <c r="B51" t="s" s="7">
+    <row r="54" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="8"/>
+      <c r="B54" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C51" t="s" s="7">
+      <c r="C54" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D51" t="s" s="7">
+      <c r="D54" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E51" t="s" s="7">
+      <c r="E54" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="52" ht="16.6" customHeight="1">
-      <c r="A52" s="8"/>
-      <c r="B52" t="s" s="7">
+    <row r="55" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="8"/>
+      <c r="B55" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="C52" t="s" s="7">
+      <c r="C55" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="D52" t="s" s="7">
+      <c r="D55" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="E52" t="s" s="7">
+      <c r="E55" s="7" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="53" ht="16.6" customHeight="1">
-      <c r="A53" s="8"/>
-      <c r="B53" t="s" s="7">
+    <row r="56" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="8"/>
+      <c r="B56" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C53" t="s" s="7">
+      <c r="C56" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="D53" t="s" s="7">
+      <c r="D56" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E53" t="s" s="7">
+      <c r="E56" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="54" ht="16.6" customHeight="1">
-      <c r="A54" s="8"/>
-      <c r="B54" t="s" s="7">
+    <row r="57" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="8"/>
+      <c r="B57" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C54" t="s" s="7">
+      <c r="C57" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D54" t="s" s="7">
+      <c r="D57" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="E54" t="s" s="7">
+      <c r="E57" s="7" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="55" ht="16.6" customHeight="1">
-      <c r="A55" s="8"/>
-      <c r="B55" t="s" s="7">
+    <row r="58" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="8"/>
+      <c r="B58" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="C55" t="s" s="7">
+      <c r="C58" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="D55" t="s" s="7">
+      <c r="D58" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="E55" t="s" s="7">
+      <c r="E58" s="7" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="56" ht="16.6" customHeight="1">
-      <c r="A56" s="8"/>
-      <c r="B56" t="s" s="7">
+    <row r="59" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="8"/>
+      <c r="B59" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="C56" t="s" s="7">
+      <c r="C59" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="D56" t="s" s="7">
+      <c r="D59" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="E56" t="s" s="7">
+      <c r="E59" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="57" ht="16.6" customHeight="1">
-      <c r="A57" s="8"/>
-      <c r="B57" t="s" s="7">
+    <row r="60" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="8"/>
+      <c r="B60" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="C57" t="s" s="7">
+      <c r="C60" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="D57" t="s" s="7">
+      <c r="D60" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="E57" t="s" s="7">
+      <c r="E60" s="7" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="58" ht="16.6" customHeight="1">
-      <c r="A58" s="8"/>
-      <c r="B58" t="s" s="7">
+    <row r="61" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="8"/>
+      <c r="B61" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="C58" t="s" s="7">
+      <c r="C61" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D58" t="s" s="7">
+      <c r="D61" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="E58" t="s" s="7">
+      <c r="E61" s="7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="59" ht="16.6" customHeight="1">
-      <c r="A59" s="8"/>
-      <c r="B59" t="s" s="7">
+    <row r="62" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="8"/>
+      <c r="B62" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="C59" t="s" s="7">
+      <c r="C62" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="D59" t="s" s="7">
+      <c r="D62" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="E59" t="s" s="7">
+      <c r="E62" s="7" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="60" ht="16.6" customHeight="1">
-      <c r="A60" s="8"/>
-      <c r="B60" t="s" s="7">
+    <row r="63" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="8"/>
+      <c r="B63" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="C60" t="s" s="7">
+      <c r="C63" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="D60" t="s" s="7">
+      <c r="D63" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="E60" t="s" s="7">
+      <c r="E63" s="7" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="61" ht="16.6" customHeight="1">
-      <c r="A61" s="8"/>
-      <c r="B61" t="s" s="7">
+    <row r="64" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="8"/>
+      <c r="B64" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="C61" t="s" s="7">
+      <c r="C64" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="D61" t="s" s="7">
+      <c r="D64" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E61" t="s" s="7">
+      <c r="E64" s="7" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="62" ht="16.6" customHeight="1">
-      <c r="A62" t="s" s="9">
+    <row r="65" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="11"/>
-    </row>
-    <row r="63" ht="16.6" customHeight="1">
-      <c r="A63" s="8"/>
-      <c r="B63" t="s" s="7">
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="11"/>
+    </row>
+    <row r="66" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="8"/>
+      <c r="B66" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="C63" t="s" s="7">
+      <c r="C66" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="D63" t="s" s="7">
+      <c r="D66" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="E63" t="s" s="7">
+      <c r="E66" s="7" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="64" ht="16.6" customHeight="1">
-      <c r="A64" s="8"/>
-      <c r="B64" t="s" s="7">
+    <row r="67" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="8"/>
+      <c r="B67" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="C64" t="s" s="7">
+      <c r="C67" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="D64" t="s" s="7">
+      <c r="D67" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="E64" t="s" s="7">
+      <c r="E67" s="7" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="65" ht="16.6" customHeight="1">
-      <c r="A65" s="8"/>
-      <c r="B65" t="s" s="7">
+    <row r="68" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="8"/>
+      <c r="B68" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="C65" t="s" s="7">
+      <c r="C68" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="D65" t="s" s="7">
+      <c r="D68" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="E65" t="s" s="7">
+      <c r="E68" s="7" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="66" ht="16.6" customHeight="1">
-      <c r="A66" s="8"/>
-      <c r="B66" t="s" s="7">
+    <row r="69" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="8"/>
+      <c r="B69" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="C66" t="s" s="7">
+      <c r="C69" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="D66" t="s" s="7">
+      <c r="D69" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="E66" t="s" s="7">
+      <c r="E69" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="67" ht="16.6" customHeight="1">
-      <c r="A67" s="8"/>
-      <c r="B67" t="s" s="7">
+    <row r="70" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="8"/>
+      <c r="B70" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="C67" t="s" s="7">
+      <c r="C70" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="D67" t="s" s="7">
+      <c r="D70" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="E67" t="s" s="7">
+      <c r="E70" s="7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="68" ht="16.6" customHeight="1">
-      <c r="A68" s="8"/>
-      <c r="B68" t="s" s="7">
+    <row r="71" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="8"/>
+      <c r="B71" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="C68" t="s" s="7">
+      <c r="C71" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D68" t="s" s="7">
+      <c r="D71" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="E68" t="s" s="7">
+      <c r="E71" s="7" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="69" ht="16.6" customHeight="1">
-      <c r="A69" s="8"/>
-      <c r="B69" t="s" s="7">
+    <row r="72" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="8"/>
+      <c r="B72" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="C69" t="s" s="7">
+      <c r="C72" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="D69" t="s" s="7">
+      <c r="D72" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="E69" t="s" s="7">
+      <c r="E72" s="7" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="70" ht="16.6" customHeight="1">
-      <c r="A70" s="8"/>
-      <c r="B70" t="s" s="7">
+    <row r="73" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="8"/>
+      <c r="B73" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="C70" t="s" s="7">
+      <c r="C73" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="D70" t="s" s="7">
+      <c r="D73" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="E70" t="s" s="7">
+      <c r="E73" s="7" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="71" ht="16.6" customHeight="1">
-      <c r="A71" s="8"/>
-      <c r="B71" t="s" s="7">
+    <row r="74" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="8"/>
+      <c r="B74" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="C71" t="s" s="7">
+      <c r="C74" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D71" t="s" s="7">
+      <c r="D74" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="E71" t="s" s="7">
+      <c r="E74" s="7" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="72" ht="17" customHeight="1">
-      <c r="A72" t="s" s="9">
+    <row r="75" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="11"/>
-    </row>
-    <row r="73" ht="17" customHeight="1">
-      <c r="A73" s="14"/>
-      <c r="B73" t="s" s="15">
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="11"/>
+    </row>
+    <row r="76" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="14"/>
+      <c r="B76" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="C73" t="s" s="15">
+      <c r="C76" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="D73" t="s" s="15">
+      <c r="D76" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="E73" t="s" s="15">
+      <c r="E76" s="15" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="74" ht="17" customHeight="1">
-      <c r="A74" s="14"/>
-      <c r="B74" t="s" s="15">
+    <row r="77" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="14"/>
+      <c r="B77" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C74" t="s" s="15">
+      <c r="C77" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="D74" t="s" s="15">
+      <c r="D77" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="E74" t="s" s="15">
+      <c r="E77" s="15" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="75" ht="17" customHeight="1">
-      <c r="A75" s="14"/>
-      <c r="B75" t="s" s="15">
+    <row r="78" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="14"/>
+      <c r="B78" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="C75" t="s" s="15">
+      <c r="C78" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="D75" t="s" s="15">
+      <c r="D78" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="E75" t="s" s="15">
+      <c r="E78" s="15" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="76" ht="17" customHeight="1">
-      <c r="A76" s="14"/>
-      <c r="B76" t="s" s="15">
+    <row r="79" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="14"/>
+      <c r="B79" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="C76" t="s" s="15">
+      <c r="C79" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="D76" t="s" s="15">
+      <c r="D79" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="E76" t="s" s="15">
+      <c r="E79" s="15" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="77" ht="17" customHeight="1">
-      <c r="A77" s="14"/>
-      <c r="B77" t="s" s="15">
+    <row r="80" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="14"/>
+      <c r="B80" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="C77" t="s" s="15">
+      <c r="C80" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="D77" t="s" s="15">
+      <c r="D80" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="E77" t="s" s="15">
+      <c r="E80" s="15" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="78" ht="17" customHeight="1">
-      <c r="A78" s="14"/>
-      <c r="B78" t="s" s="15">
+    <row r="81" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="14"/>
+      <c r="B81" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="C78" t="s" s="15">
+      <c r="C81" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="D78" t="s" s="15">
+      <c r="D81" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="E78" t="s" s="15">
+      <c r="E81" s="15" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="79" ht="17" customHeight="1">
-      <c r="A79" s="14"/>
-      <c r="B79" t="s" s="15">
+    <row r="82" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="14"/>
+      <c r="B82" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C79" t="s" s="15">
+      <c r="C82" s="15" t="s">
         <v>285</v>
       </c>
-      <c r="D79" t="s" s="15">
+      <c r="D82" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="E79" t="s" s="15">
+      <c r="E82" s="15" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="80" ht="17" customHeight="1">
-      <c r="A80" s="14"/>
-      <c r="B80" t="s" s="15">
+    <row r="83" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="14"/>
+      <c r="B83" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="C80" t="s" s="15">
+      <c r="C83" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="D80" t="s" s="15">
+      <c r="D83" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="E80" t="s" s="15">
+      <c r="E83" s="15" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="81" ht="17" customHeight="1">
-      <c r="A81" s="14"/>
-      <c r="B81" t="s" s="15">
+    <row r="84" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="14"/>
+      <c r="B84" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="C81" t="s" s="15">
+      <c r="C84" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="D81" t="s" s="15">
+      <c r="D84" s="15" t="s">
         <v>294</v>
       </c>
-      <c r="E81" t="s" s="15">
+      <c r="E84" s="15" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="82" ht="17" customHeight="1">
-      <c r="A82" s="14"/>
-      <c r="B82" t="s" s="15">
+    <row r="85" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="14"/>
+      <c r="B85" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="C82" t="s" s="15">
+      <c r="C85" s="15" t="s">
         <v>297</v>
       </c>
-      <c r="D82" t="s" s="15">
+      <c r="D85" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="E82" t="s" s="15">
+      <c r="E85" s="15" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="83" ht="17" customHeight="1">
-      <c r="A83" s="14"/>
-      <c r="B83" t="s" s="15">
+    <row r="86" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="14"/>
+      <c r="B86" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="C83" t="s" s="15">
+      <c r="C86" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="D83" t="s" s="15">
+      <c r="D86" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="E83" t="s" s="15">
+      <c r="E86" s="15" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="84" ht="17" customHeight="1">
-      <c r="A84" s="14"/>
-      <c r="B84" t="s" s="15">
+    <row r="87" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="14"/>
+      <c r="B87" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="C84" t="s" s="15">
+      <c r="C87" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="D84" t="s" s="15">
+      <c r="D87" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="E84" t="s" s="15">
+      <c r="E87" s="15" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="85" ht="17" customHeight="1">
-      <c r="A85" s="14"/>
-      <c r="B85" s="15"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
-      <c r="E85" s="14"/>
-    </row>
-    <row r="86" ht="17" customHeight="1">
-      <c r="A86" s="14"/>
-      <c r="B86" s="15"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="14"/>
-      <c r="E86" s="14"/>
-    </row>
-    <row r="87" ht="17" customHeight="1">
-      <c r="A87" s="14"/>
-      <c r="B87" s="16"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-    </row>
-    <row r="88" ht="17" customHeight="1">
+    <row r="88" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="14"/>
-      <c r="B88" s="17"/>
+      <c r="B88" s="15"/>
       <c r="C88" s="14"/>
       <c r="D88" s="14"/>
       <c r="E88" s="14"/>
     </row>
-    <row r="89" ht="17" customHeight="1">
+    <row r="89" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="14"/>
-      <c r="B89" s="17"/>
+      <c r="B89" s="15"/>
       <c r="C89" s="14"/>
       <c r="D89" s="14"/>
       <c r="E89" s="14"/>
     </row>
-    <row r="90" ht="17" customHeight="1">
+    <row r="90" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="14"/>
-      <c r="B90" s="17"/>
+      <c r="B90" s="16"/>
       <c r="C90" s="14"/>
       <c r="D90" s="14"/>
       <c r="E90" s="14"/>
     </row>
-    <row r="91" ht="17" customHeight="1">
+    <row r="91" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="14"/>
       <c r="B91" s="17"/>
       <c r="C91" s="14"/>
       <c r="D91" s="14"/>
       <c r="E91" s="14"/>
     </row>
-    <row r="92" ht="17" customHeight="1">
+    <row r="92" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="14"/>
       <c r="B92" s="17"/>
       <c r="C92" s="14"/>
       <c r="D92" s="14"/>
       <c r="E92" s="14"/>
     </row>
-    <row r="93" ht="17" customHeight="1">
+    <row r="93" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="14"/>
       <c r="B93" s="17"/>
       <c r="C93" s="14"/>
       <c r="D93" s="14"/>
       <c r="E93" s="14"/>
     </row>
-    <row r="94" ht="17" customHeight="1">
+    <row r="94" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="14"/>
       <c r="B94" s="17"/>
       <c r="C94" s="14"/>
       <c r="D94" s="14"/>
       <c r="E94" s="14"/>
     </row>
-    <row r="95" ht="17" customHeight="1">
+    <row r="95" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="14"/>
       <c r="B95" s="17"/>
       <c r="C95" s="14"/>
       <c r="D95" s="14"/>
       <c r="E95" s="14"/>
     </row>
-    <row r="96" ht="17" customHeight="1">
+    <row r="96" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="14"/>
       <c r="B96" s="17"/>
       <c r="C96" s="14"/>
       <c r="D96" s="14"/>
       <c r="E96" s="14"/>
     </row>
-    <row r="97" ht="17" customHeight="1">
+    <row r="97" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="14"/>
       <c r="B97" s="17"/>
       <c r="C97" s="14"/>
       <c r="D97" s="14"/>
       <c r="E97" s="14"/>
     </row>
-    <row r="98" ht="17" customHeight="1">
+    <row r="98" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="14"/>
       <c r="B98" s="17"/>
       <c r="C98" s="14"/>
       <c r="D98" s="14"/>
       <c r="E98" s="14"/>
     </row>
-    <row r="99" ht="17" customHeight="1">
+    <row r="99" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="14"/>
       <c r="B99" s="17"/>
       <c r="C99" s="14"/>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
     </row>
-    <row r="100" ht="17" customHeight="1">
+    <row r="100" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="14"/>
       <c r="B100" s="17"/>
       <c r="C100" s="14"/>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
     </row>
-    <row r="101" ht="17" customHeight="1">
+    <row r="101" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="14"/>
       <c r="B101" s="17"/>
       <c r="C101" s="14"/>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
     </row>
-    <row r="102" ht="17" customHeight="1">
+    <row r="102" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="14"/>
       <c r="B102" s="17"/>
       <c r="C102" s="14"/>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
     </row>
-    <row r="103" ht="17" customHeight="1">
+    <row r="103" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="14"/>
       <c r="B103" s="17"/>
       <c r="C103" s="14"/>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
     </row>
-    <row r="104" ht="17" customHeight="1">
+    <row r="104" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="14"/>
       <c r="B104" s="17"/>
       <c r="C104" s="14"/>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
     </row>
-    <row r="105" ht="17" customHeight="1">
+    <row r="105" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="14"/>
       <c r="B105" s="17"/>
       <c r="C105" s="14"/>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
     </row>
-    <row r="106" ht="17" customHeight="1">
+    <row r="106" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="14"/>
       <c r="B106" s="17"/>
       <c r="C106" s="14"/>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
     </row>
-    <row r="107" ht="17" customHeight="1">
+    <row r="107" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="14"/>
       <c r="B107" s="17"/>
       <c r="C107" s="14"/>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
     </row>
-    <row r="108" ht="17" customHeight="1">
+    <row r="108" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="14"/>
       <c r="B108" s="17"/>
       <c r="C108" s="14"/>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
     </row>
-    <row r="109" ht="17" customHeight="1">
+    <row r="109" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="14"/>
       <c r="B109" s="17"/>
       <c r="C109" s="14"/>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
     </row>
-    <row r="110" ht="17" customHeight="1">
+    <row r="110" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="14"/>
       <c r="B110" s="17"/>
       <c r="C110" s="14"/>
       <c r="D110" s="14"/>
       <c r="E110" s="14"/>
     </row>
-    <row r="111" ht="17" customHeight="1">
+    <row r="111" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="14"/>
       <c r="B111" s="17"/>
       <c r="C111" s="14"/>
       <c r="D111" s="14"/>
       <c r="E111" s="14"/>
     </row>
-    <row r="112" ht="17" customHeight="1">
+    <row r="112" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="14"/>
       <c r="B112" s="17"/>
       <c r="C112" s="14"/>
       <c r="D112" s="14"/>
       <c r="E112" s="14"/>
     </row>
-    <row r="113" ht="17" customHeight="1">
+    <row r="113" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="14"/>
       <c r="B113" s="17"/>
       <c r="C113" s="14"/>
       <c r="D113" s="14"/>
       <c r="E113" s="14"/>
     </row>
-    <row r="114" ht="17" customHeight="1">
+    <row r="114" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="14"/>
       <c r="B114" s="17"/>
       <c r="C114" s="14"/>
       <c r="D114" s="14"/>
       <c r="E114" s="14"/>
     </row>
-    <row r="115" ht="17" customHeight="1">
+    <row r="115" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="14"/>
       <c r="B115" s="17"/>
       <c r="C115" s="14"/>
       <c r="D115" s="14"/>
       <c r="E115" s="14"/>
     </row>
-    <row r="116" ht="17" customHeight="1">
+    <row r="116" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="14"/>
       <c r="B116" s="17"/>
       <c r="C116" s="14"/>
       <c r="D116" s="14"/>
       <c r="E116" s="14"/>
     </row>
-    <row r="117" ht="17" customHeight="1">
+    <row r="117" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="14"/>
       <c r="B117" s="17"/>
       <c r="C117" s="14"/>
       <c r="D117" s="14"/>
       <c r="E117" s="14"/>
     </row>
-    <row r="118" ht="17" customHeight="1">
+    <row r="118" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="14"/>
       <c r="B118" s="17"/>
       <c r="C118" s="14"/>
       <c r="D118" s="14"/>
       <c r="E118" s="14"/>
     </row>
-    <row r="119" ht="17" customHeight="1">
+    <row r="119" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="14"/>
       <c r="B119" s="17"/>
       <c r="C119" s="14"/>
       <c r="D119" s="14"/>
       <c r="E119" s="14"/>
     </row>
-    <row r="120" ht="17" customHeight="1">
+    <row r="120" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="14"/>
       <c r="B120" s="17"/>
       <c r="C120" s="14"/>
       <c r="D120" s="14"/>
       <c r="E120" s="14"/>
     </row>
-    <row r="121" ht="17" customHeight="1">
+    <row r="121" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="14"/>
       <c r="B121" s="17"/>
       <c r="C121" s="14"/>
       <c r="D121" s="14"/>
       <c r="E121" s="14"/>
     </row>
-    <row r="122" ht="17" customHeight="1">
+    <row r="122" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="14"/>
       <c r="B122" s="17"/>
       <c r="C122" s="14"/>
       <c r="D122" s="14"/>
       <c r="E122" s="14"/>
     </row>
-    <row r="123" ht="17" customHeight="1">
+    <row r="123" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="14"/>
       <c r="B123" s="17"/>
       <c r="C123" s="14"/>
       <c r="D123" s="14"/>
       <c r="E123" s="14"/>
     </row>
-    <row r="124" ht="17" customHeight="1">
+    <row r="124" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="14"/>
       <c r="B124" s="17"/>
       <c r="C124" s="14"/>
       <c r="D124" s="14"/>
       <c r="E124" s="14"/>
     </row>
-    <row r="125" ht="17" customHeight="1">
+    <row r="125" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="14"/>
       <c r="B125" s="17"/>
       <c r="C125" s="14"/>
       <c r="D125" s="14"/>
       <c r="E125" s="14"/>
     </row>
-    <row r="126" ht="17" customHeight="1">
+    <row r="126" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="14"/>
       <c r="B126" s="17"/>
       <c r="C126" s="14"/>
       <c r="D126" s="14"/>
       <c r="E126" s="14"/>
     </row>
-    <row r="127" ht="17" customHeight="1">
+    <row r="127" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="14"/>
       <c r="B127" s="17"/>
       <c r="C127" s="14"/>
       <c r="D127" s="14"/>
       <c r="E127" s="14"/>
     </row>
-    <row r="128" ht="17" customHeight="1">
+    <row r="128" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="14"/>
       <c r="B128" s="17"/>
       <c r="C128" s="14"/>
       <c r="D128" s="14"/>
       <c r="E128" s="14"/>
     </row>
-    <row r="129" ht="17" customHeight="1">
+    <row r="129" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="14"/>
       <c r="B129" s="17"/>
       <c r="C129" s="14"/>
       <c r="D129" s="14"/>
       <c r="E129" s="14"/>
     </row>
-    <row r="130" ht="17" customHeight="1">
+    <row r="130" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="14"/>
       <c r="B130" s="17"/>
       <c r="C130" s="14"/>
       <c r="D130" s="14"/>
       <c r="E130" s="14"/>
     </row>
-    <row r="131" ht="17" customHeight="1">
+    <row r="131" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="14"/>
       <c r="B131" s="17"/>
       <c r="C131" s="14"/>
       <c r="D131" s="14"/>
       <c r="E131" s="14"/>
     </row>
-    <row r="132" ht="17" customHeight="1">
+    <row r="132" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="14"/>
       <c r="B132" s="17"/>
       <c r="C132" s="14"/>
       <c r="D132" s="14"/>
       <c r="E132" s="14"/>
     </row>
-    <row r="133" ht="17" customHeight="1">
+    <row r="133" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="14"/>
       <c r="B133" s="17"/>
       <c r="C133" s="14"/>
       <c r="D133" s="14"/>
       <c r="E133" s="14"/>
     </row>
-    <row r="134" ht="17" customHeight="1">
+    <row r="134" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="14"/>
       <c r="B134" s="17"/>
       <c r="C134" s="14"/>
       <c r="D134" s="14"/>
       <c r="E134" s="14"/>
     </row>
-    <row r="135" ht="17" customHeight="1">
+    <row r="135" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="14"/>
       <c r="B135" s="17"/>
       <c r="C135" s="14"/>
       <c r="D135" s="14"/>
       <c r="E135" s="14"/>
     </row>
-    <row r="136" ht="17" customHeight="1">
+    <row r="136" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="14"/>
       <c r="B136" s="17"/>
       <c r="C136" s="14"/>
       <c r="D136" s="14"/>
       <c r="E136" s="14"/>
     </row>
-    <row r="137" ht="17" customHeight="1">
+    <row r="137" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="14"/>
       <c r="B137" s="17"/>
       <c r="C137" s="14"/>
       <c r="D137" s="14"/>
       <c r="E137" s="14"/>
     </row>
-    <row r="138" ht="17" customHeight="1">
+    <row r="138" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="14"/>
       <c r="B138" s="17"/>
       <c r="C138" s="14"/>
       <c r="D138" s="14"/>
       <c r="E138" s="14"/>
     </row>
-    <row r="139" ht="17" customHeight="1">
+    <row r="139" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="14"/>
       <c r="B139" s="17"/>
       <c r="C139" s="14"/>
       <c r="D139" s="14"/>
       <c r="E139" s="14"/>
     </row>
-    <row r="140" ht="17" customHeight="1">
+    <row r="140" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="14"/>
       <c r="B140" s="17"/>
       <c r="C140" s="14"/>
       <c r="D140" s="14"/>
       <c r="E140" s="14"/>
     </row>
-    <row r="141" ht="17" customHeight="1">
+    <row r="141" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="14"/>
       <c r="B141" s="17"/>
       <c r="C141" s="14"/>
       <c r="D141" s="14"/>
       <c r="E141" s="14"/>
     </row>
-    <row r="142" ht="17" customHeight="1">
+    <row r="142" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="14"/>
       <c r="B142" s="17"/>
       <c r="C142" s="14"/>
       <c r="D142" s="14"/>
       <c r="E142" s="14"/>
     </row>
-    <row r="143" ht="17" customHeight="1">
+    <row r="143" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="14"/>
       <c r="B143" s="17"/>
       <c r="C143" s="14"/>
       <c r="D143" s="14"/>
       <c r="E143" s="14"/>
     </row>
-    <row r="144" ht="17" customHeight="1">
+    <row r="144" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="14"/>
       <c r="B144" s="17"/>
       <c r="C144" s="14"/>
       <c r="D144" s="14"/>
       <c r="E144" s="14"/>
     </row>
-    <row r="145" ht="17" customHeight="1">
+    <row r="145" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="14"/>
       <c r="B145" s="17"/>
       <c r="C145" s="14"/>
       <c r="D145" s="14"/>
       <c r="E145" s="14"/>
     </row>
-    <row r="146" ht="17" customHeight="1">
+    <row r="146" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="14"/>
       <c r="B146" s="17"/>
       <c r="C146" s="14"/>
       <c r="D146" s="14"/>
       <c r="E146" s="14"/>
     </row>
-    <row r="147" ht="17" customHeight="1">
+    <row r="147" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="14"/>
       <c r="B147" s="17"/>
       <c r="C147" s="14"/>
       <c r="D147" s="14"/>
       <c r="E147" s="14"/>
     </row>
-    <row r="148" ht="17" customHeight="1">
+    <row r="148" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="14"/>
       <c r="B148" s="17"/>
       <c r="C148" s="14"/>
       <c r="D148" s="14"/>
       <c r="E148" s="14"/>
     </row>
-    <row r="149" ht="17" customHeight="1">
+    <row r="149" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="14"/>
       <c r="B149" s="17"/>
       <c r="C149" s="14"/>
       <c r="D149" s="14"/>
       <c r="E149" s="14"/>
     </row>
-    <row r="150" ht="17" customHeight="1">
+    <row r="150" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="14"/>
       <c r="B150" s="17"/>
       <c r="C150" s="14"/>
       <c r="D150" s="14"/>
       <c r="E150" s="14"/>
     </row>
-    <row r="151" ht="17" customHeight="1">
+    <row r="151" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="14"/>
       <c r="B151" s="17"/>
       <c r="C151" s="14"/>
       <c r="D151" s="14"/>
       <c r="E151" s="14"/>
     </row>
-    <row r="152" ht="17" customHeight="1">
+    <row r="152" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="14"/>
       <c r="B152" s="17"/>
       <c r="C152" s="14"/>
       <c r="D152" s="14"/>
       <c r="E152" s="14"/>
     </row>
-    <row r="153" ht="17" customHeight="1">
+    <row r="153" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="14"/>
       <c r="B153" s="17"/>
       <c r="C153" s="14"/>
       <c r="D153" s="14"/>
       <c r="E153" s="14"/>
     </row>
-    <row r="154" ht="17" customHeight="1">
+    <row r="154" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="14"/>
       <c r="B154" s="17"/>
       <c r="C154" s="14"/>
       <c r="D154" s="14"/>
       <c r="E154" s="14"/>
     </row>
-    <row r="155" ht="17" customHeight="1">
+    <row r="155" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="14"/>
       <c r="B155" s="17"/>
       <c r="C155" s="14"/>
       <c r="D155" s="14"/>
       <c r="E155" s="14"/>
     </row>
-    <row r="156" ht="17" customHeight="1">
+    <row r="156" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="14"/>
       <c r="B156" s="17"/>
       <c r="C156" s="14"/>
       <c r="D156" s="14"/>
       <c r="E156" s="14"/>
     </row>
-    <row r="157" ht="17" customHeight="1">
+    <row r="157" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="14"/>
       <c r="B157" s="17"/>
       <c r="C157" s="14"/>
       <c r="D157" s="14"/>
       <c r="E157" s="14"/>
     </row>
-    <row r="158" ht="17" customHeight="1">
+    <row r="158" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="14"/>
       <c r="B158" s="17"/>
       <c r="C158" s="14"/>
       <c r="D158" s="14"/>
       <c r="E158" s="14"/>
     </row>
-    <row r="159" ht="17" customHeight="1">
+    <row r="159" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="14"/>
       <c r="B159" s="17"/>
       <c r="C159" s="14"/>
       <c r="D159" s="14"/>
       <c r="E159" s="14"/>
     </row>
-    <row r="160" ht="17" customHeight="1">
+    <row r="160" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="14"/>
       <c r="B160" s="17"/>
       <c r="C160" s="14"/>
       <c r="D160" s="14"/>
       <c r="E160" s="14"/>
     </row>
-    <row r="161" ht="17" customHeight="1">
+    <row r="161" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="14"/>
       <c r="B161" s="17"/>
       <c r="C161" s="14"/>
       <c r="D161" s="14"/>
       <c r="E161" s="14"/>
     </row>
+    <row r="162" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="14"/>
+      <c r="B162" s="17"/>
+      <c r="C162" s="14"/>
+      <c r="D162" s="14"/>
+      <c r="E162" s="14"/>
+    </row>
+    <row r="163" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="14"/>
+      <c r="B163" s="17"/>
+      <c r="C163" s="14"/>
+      <c r="D163" s="14"/>
+      <c r="E163" s="14"/>
+    </row>
+    <row r="164" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="14"/>
+      <c r="B164" s="17"/>
+      <c r="C164" s="14"/>
+      <c r="D164" s="14"/>
+      <c r="E164" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
In map view, added a way to edit drives even more easily. Can now delete a whole interval from Point1 to Point2 and  can split an interval (adding new point in between)
</commit_message>
<xml_diff>
--- a/gpstracker_languages.xlsx
+++ b/gpstracker_languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gt/Documents/MainProjects/DrivesApp/SWIFT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C80DBC-4DF4-9A46-BF8F-318C9E3A5F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CDF218-342B-C84A-9D49-1B5380A6CBE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="500" windowWidth="24720" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="333">
   <si>
     <t>COMMENT</t>
   </si>
@@ -955,15 +955,6 @@
     <t>Pabeigt</t>
   </si>
   <si>
-    <t>move_button_title</t>
-  </si>
-  <si>
-    <t>Move</t>
-  </si>
-  <si>
-    <t>Pārvietot</t>
-  </si>
-  <si>
     <t>edit_button_title</t>
   </si>
   <si>
@@ -976,13 +967,58 @@
     <t>Сделанный</t>
   </si>
   <si>
-    <t>Переместить точку</t>
-  </si>
-  <si>
     <t>Редактировать</t>
   </si>
   <si>
     <t>Внимание</t>
+  </si>
+  <si>
+    <t>Select P1-P2</t>
+  </si>
+  <si>
+    <t>Delete P1-P2</t>
+  </si>
+  <si>
+    <t>Split</t>
+  </si>
+  <si>
+    <t>Move P1</t>
+  </si>
+  <si>
+    <t>map_move_point</t>
+  </si>
+  <si>
+    <t>map_split_interval</t>
+  </si>
+  <si>
+    <t>map_delete_interval</t>
+  </si>
+  <si>
+    <t>map_select_interval</t>
+  </si>
+  <si>
+    <t>Pārvietot P1</t>
+  </si>
+  <si>
+    <t>Sadalīt</t>
+  </si>
+  <si>
+    <t>Dzēst P1-P2</t>
+  </si>
+  <si>
+    <t>Iezīmēt P1-P2</t>
+  </si>
+  <si>
+    <t>Переместить P1</t>
+  </si>
+  <si>
+    <t>Удалить P1-P2</t>
+  </si>
+  <si>
+    <t>Разделить</t>
+  </si>
+  <si>
+    <t>Выделять P1-P2</t>
   </si>
 </sst>
 </file>
@@ -2336,10 +2372,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E167"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2514,7 +2550,7 @@
         <v>41</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2529,7 +2565,7 @@
         <v>310</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2544,1123 +2580,1147 @@
         <v>313</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="7" t="s">
-        <v>314</v>
+        <v>42</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>315</v>
+        <v>43</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>316</v>
+        <v>44</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>319</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>45</v>
-      </c>
+      <c r="A15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>58</v>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>62</v>
-      </c>
+      <c r="A20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
+      <c r="A21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>68</v>
+      <c r="A22" s="8"/>
+      <c r="B22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="7" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="7" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="7" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="7" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="7" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="7" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="7" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
       <c r="B35" s="7" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="7" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
       <c r="B37" s="7" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="7" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
       <c r="B39" s="7" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="A40" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="11"/>
     </row>
     <row r="41" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="7" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8"/>
       <c r="B43" s="7" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="7" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8"/>
       <c r="B45" s="7" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8"/>
       <c r="B46" s="7" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8"/>
       <c r="B47" s="7" t="s">
-        <v>159</v>
+        <v>324</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>160</v>
+        <v>317</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>161</v>
+        <v>328</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>162</v>
+        <v>332</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
       <c r="B48" s="7" t="s">
-        <v>163</v>
+        <v>323</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>164</v>
+        <v>318</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>165</v>
+        <v>327</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>166</v>
+        <v>330</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="11"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="50" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8"/>
       <c r="B50" s="7" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>169</v>
+        <v>320</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>170</v>
+        <v>325</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>171</v>
+        <v>329</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8"/>
       <c r="B51" s="7" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
-      <c r="B52" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>179</v>
-      </c>
+      <c r="A52" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="11"/>
     </row>
     <row r="53" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="8"/>
       <c r="B53" s="7" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="8"/>
       <c r="B54" s="7" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="8"/>
       <c r="B55" s="7" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="8"/>
       <c r="B56" s="7" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="8"/>
       <c r="B57" s="7" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8"/>
       <c r="B58" s="7" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8"/>
       <c r="B59" s="7" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8"/>
       <c r="B60" s="7" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="8"/>
       <c r="B61" s="7" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
       <c r="B62" s="7" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8"/>
       <c r="B63" s="7" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="8"/>
       <c r="B64" s="7" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="11"/>
+      <c r="A65" s="8"/>
+      <c r="B65" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="66" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="8"/>
       <c r="B66" s="7" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="8"/>
       <c r="B67" s="7" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="8"/>
-      <c r="B68" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>234</v>
-      </c>
+      <c r="A68" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="11"/>
     </row>
     <row r="69" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8"/>
       <c r="B69" s="7" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="8"/>
       <c r="B70" s="7" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="8"/>
       <c r="B71" s="7" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="8"/>
       <c r="B72" s="7" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="8"/>
       <c r="B73" s="7" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="8"/>
       <c r="B74" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="8"/>
+      <c r="B75" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="8"/>
+      <c r="B76" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="8"/>
+      <c r="B77" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="C77" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D77" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="E74" s="7" t="s">
+      <c r="E77" s="7" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="9" t="s">
+    <row r="78" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-      <c r="E75" s="11"/>
-    </row>
-    <row r="76" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="14"/>
-      <c r="B76" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="C76" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="D76" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="E76" s="15" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="14"/>
-      <c r="B77" s="15" t="s">
-        <v>264</v>
-      </c>
-      <c r="C77" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="D77" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="E77" s="15" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="14"/>
-      <c r="B78" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="C78" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="D78" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="E78" s="15" t="s">
-        <v>271</v>
-      </c>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="11"/>
     </row>
     <row r="79" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="14"/>
       <c r="B79" s="15" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="D79" s="15" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="E79" s="15" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="14"/>
       <c r="B80" s="15" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="D80" s="15" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="E80" s="15" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="14"/>
       <c r="B81" s="15" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="D81" s="15" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="E81" s="15" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="14"/>
       <c r="B82" s="15" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="D82" s="15" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="E82" s="15" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="14"/>
       <c r="B83" s="15" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="D83" s="15" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="E83" s="15" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="14"/>
       <c r="B84" s="15" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="D84" s="15" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="E84" s="15" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="14"/>
       <c r="B85" s="15" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="D85" s="15" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="E85" s="15" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="14"/>
       <c r="B86" s="15" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="D86" s="15" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="E86" s="15" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="14"/>
       <c r="B87" s="15" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="D87" s="15" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="E87" s="15" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="14"/>
-      <c r="B88" s="15"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="14"/>
+      <c r="B88" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="E88" s="15" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="89" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="14"/>
-      <c r="B89" s="15"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
+      <c r="B89" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="E89" s="15" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="90" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="14"/>
-      <c r="B90" s="16"/>
-      <c r="C90" s="14"/>
-      <c r="D90" s="14"/>
-      <c r="E90" s="14"/>
+      <c r="B90" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="C90" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="E90" s="15" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="91" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="14"/>
-      <c r="B91" s="17"/>
+      <c r="B91" s="15"/>
       <c r="C91" s="14"/>
       <c r="D91" s="14"/>
       <c r="E91" s="14"/>
     </row>
     <row r="92" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="14"/>
-      <c r="B92" s="17"/>
+      <c r="B92" s="15"/>
       <c r="C92" s="14"/>
       <c r="D92" s="14"/>
       <c r="E92" s="14"/>
     </row>
     <row r="93" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="14"/>
-      <c r="B93" s="17"/>
+      <c r="B93" s="16"/>
       <c r="C93" s="14"/>
       <c r="D93" s="14"/>
       <c r="E93" s="14"/>
@@ -4161,6 +4221,27 @@
       <c r="C164" s="14"/>
       <c r="D164" s="14"/>
       <c r="E164" s="14"/>
+    </row>
+    <row r="165" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="14"/>
+      <c r="B165" s="17"/>
+      <c r="C165" s="14"/>
+      <c r="D165" s="14"/>
+      <c r="E165" s="14"/>
+    </row>
+    <row r="166" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="14"/>
+      <c r="B166" s="17"/>
+      <c r="C166" s="14"/>
+      <c r="D166" s="14"/>
+      <c r="E166" s="14"/>
+    </row>
+    <row r="167" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="14"/>
+      <c r="B167" s="17"/>
+      <c r="C167" s="14"/>
+      <c r="D167" s="14"/>
+      <c r="E167" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>